<commit_message>
DA input for part 2
</commit_message>
<xml_diff>
--- a/data_analysis.xlsx
+++ b/data_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edrick\PycharmProjects\sustainbale_econ_research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF26C3FD-F84A-4E7E-9356-A18FB5F3A073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1A28A8-8337-4388-9E88-3F4631B8FC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{1B299115-941F-47A3-BD92-06D603FEB45D}"/>
   </bookViews>
@@ -16609,10 +16609,10 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M46" sqref="M46"/>
+      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>